<commit_message>
Feature : 미연시 bgm 작업
</commit_message>
<xml_diff>
--- a/Download/Assets/Resources/4. Data/1. VisualNovel/Dialogs/Dialogs_Day3At.xlsx
+++ b/Download/Assets/Resources/4. Data/1. VisualNovel/Dialogs/Dialogs_Day3At.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zenu0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Download_Project\Download\Assets\Resources\4. Data\1. VisualNovel\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2885EA-1527-416A-AC87-A592C39E8762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E1EA2C-7F36-492D-9DB1-9324F1866D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="7" xr2:uid="{49FB8DDA-CC9A-4F10-83A2-6EE5D727B386}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="760" activeTab="7" xr2:uid="{49FB8DDA-CC9A-4F10-83A2-6EE5D727B386}"/>
   </bookViews>
   <sheets>
     <sheet name="S00_11_Fail" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="282">
   <si>
     <t>dialogType</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2223,13 +2223,49 @@
   <si>
     <t>{KI01}</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MI01</t>
+  </si>
+  <si>
+    <t>SA01</t>
+  </si>
+  <si>
+    <t>SA01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SA04</t>
+  </si>
+  <si>
+    <t>KI04</t>
+  </si>
+  <si>
+    <t>KI03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KI01</t>
+  </si>
+  <si>
+    <t>KI05</t>
+  </si>
+  <si>
+    <t>KI06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bgm</t>
+  </si>
+  <si>
+    <t>effect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2325,6 +2361,31 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF657C9D"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2456,7 +2517,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2529,11 +2590,20 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="109">
     <dxf>
       <fill>
         <patternFill>
@@ -3068,12 +3138,12 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
       </font>
     </dxf>
     <dxf>
@@ -3085,11 +3155,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="3" tint="0.24994659260841701"/>
       </font>
     </dxf>
@@ -3106,11 +3171,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color theme="3" tint="0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.89996032593768116"/>
@@ -3119,12 +3179,12 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="3" tint="0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
@@ -3135,6 +3195,64 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="3" tint="0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF657C9D"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEBEDF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF657C9D"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEBEDF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
@@ -3144,14 +3262,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.89996032593768116"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3165,7 +3276,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3179,6 +3297,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -3193,21 +3318,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3229,13 +3340,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3258,9 +3362,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3298,7 +3402,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3404,7 +3508,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3546,7 +3650,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3554,21 +3658,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8247A8-D7F3-438B-95A1-19D838F3F847}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="15.19921875" customWidth="1"/>
     <col min="6" max="6" width="53" customWidth="1"/>
     <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="8" max="8" width="18.19921875" customWidth="1"/>
+    <col min="10" max="10" width="18.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3594,31 +3699,37 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3626,7 +3737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3645,11 +3756,12 @@
       <c r="H3" t="s">
         <v>222</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="I3" s="24"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3668,11 +3780,12 @@
       <c r="H4" t="s">
         <v>222</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="I4" s="25"/>
       <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3691,11 +3804,12 @@
       <c r="H5" t="s">
         <v>222</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="I5" s="25"/>
       <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3714,11 +3828,12 @@
       <c r="H6" t="s">
         <v>222</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="I6" s="25"/>
       <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3737,11 +3852,12 @@
       <c r="H7" t="s">
         <v>222</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="I7" s="26"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3760,11 +3876,12 @@
       <c r="H8" t="s">
         <v>264</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="I8" s="25"/>
       <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3783,11 +3900,15 @@
       <c r="H9" t="s">
         <v>264</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="I9" s="25"/>
+      <c r="J9" t="s">
+        <v>271</v>
+      </c>
       <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3806,11 +3927,12 @@
       <c r="H10" t="s">
         <v>264</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="I10" s="25"/>
       <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3829,11 +3951,12 @@
       <c r="H11" t="s">
         <v>264</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="I11" s="25"/>
       <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3852,11 +3975,12 @@
       <c r="H12" t="s">
         <v>222</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="I12" s="24"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3875,11 +3999,12 @@
       <c r="H13" t="s">
         <v>265</v>
       </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="I13" s="25"/>
       <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3898,11 +4023,15 @@
       <c r="H14" t="s">
         <v>265</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="I14" s="25"/>
+      <c r="J14" t="s">
+        <v>273</v>
+      </c>
       <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1</v>
       </c>
@@ -3921,11 +4050,12 @@
       <c r="H15" t="s">
         <v>265</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="I15" s="25"/>
       <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3944,11 +4074,15 @@
       <c r="H16" t="s">
         <v>222</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="I16" s="25"/>
+      <c r="J16" t="s">
+        <v>230</v>
+      </c>
       <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3967,11 +4101,12 @@
       <c r="H17" t="s">
         <v>222</v>
       </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="I17" s="25"/>
       <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3990,11 +4125,12 @@
       <c r="H18" t="s">
         <v>222</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="I18" s="25"/>
       <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>1</v>
       </c>
@@ -4013,11 +4149,12 @@
       <c r="H19" t="s">
         <v>222</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="I19" s="25"/>
       <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>1</v>
       </c>
@@ -4036,11 +4173,12 @@
       <c r="H20" t="s">
         <v>222</v>
       </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="I20" s="26"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>0</v>
       </c>
@@ -4054,102 +4192,124 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="102" priority="48" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="108" priority="55" operator="containsText" text="0">
+      <formula>NOT(ISERROR(SEARCH("0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="107" priority="54" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="49" operator="containsText" text="0">
-      <formula>NOT(ISERROR(SEARCH("0",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A21">
-    <cfRule type="containsText" dxfId="100" priority="33" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="106" priority="40" operator="containsText" text="0">
+      <formula>NOT(ISERROR(SEARCH("0",A3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="39" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="34" operator="containsText" text="0">
-      <formula>NOT(ISERROR(SEARCH("0",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="containsText" dxfId="98" priority="45" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="104" priority="51" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="46" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="103" priority="52" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="47" operator="containsText" text="0">
+    <cfRule type="containsText" dxfId="102" priority="53" operator="containsText" text="0">
       <formula>NOT(ISERROR(SEARCH("0",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="95" priority="35" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="101" priority="43" operator="containsText" text="0">
+      <formula>NOT(ISERROR(SEARCH("0",D21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="42" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",D21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="41" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",D21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="36" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",D21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="37" operator="containsText" text="0">
-      <formula>NOT(ISERROR(SEARCH("0",D21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E20">
-    <cfRule type="containsText" dxfId="92" priority="13" operator="containsText" text="나레이션">
+    <cfRule type="containsText" dxfId="98" priority="20" operator="containsText" text="히나">
+      <formula>NOT(ISERROR(SEARCH("히나",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="19" operator="containsText" text="나레이션">
       <formula>NOT(ISERROR(SEARCH("나레이션",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="14" operator="containsText" text="히나">
-      <formula>NOT(ISERROR(SEARCH("히나",E3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="15" operator="containsText" text="아야카">
+    <cfRule type="containsText" dxfId="96" priority="23" operator="containsText" text="{{PLAYER_NAME}}">
+      <formula>NOT(ISERROR(SEARCH("{{PLAYER_NAME}}",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="95" priority="22" operator="containsText" text="미나츠">
+      <formula>NOT(ISERROR(SEARCH("미나츠",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="21" operator="containsText" text="아야카">
       <formula>NOT(ISERROR(SEARCH("아야카",E3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="16" operator="containsText" text="미나츠">
-      <formula>NOT(ISERROR(SEARCH("미나츠",E3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="17" operator="containsText" text="{{PLAYER_NAME}}">
-      <formula>NOT(ISERROR(SEARCH("{{PLAYER_NAME}}",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="containsText" dxfId="87" priority="4" operator="containsText" text="MI">
+    <cfRule type="containsText" dxfId="93" priority="4" operator="containsText" text="MI">
       <formula>NOT(ISERROR(SEARCH("MI",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="5" operator="containsText" text=".">
+    <cfRule type="containsText" dxfId="92" priority="5" operator="containsText" text=".">
       <formula>NOT(ISERROR(SEARCH(".",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="6" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="91" priority="6" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",I8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="containsText" dxfId="84" priority="1" operator="containsText" text="MI">
+    <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",I11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="MI">
       <formula>NOT(ISERROR(SEARCH("MI",I11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="2" operator="containsText" text=".">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text=".">
       <formula>NOT(ISERROR(SEARCH(".",I11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="3" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",I11)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J20">
-    <cfRule type="containsText" dxfId="81" priority="10" operator="containsText" text="SA">
-      <formula>NOT(ISERROR(SEARCH("SA",J3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="11" operator="containsText" text=".">
-      <formula>NOT(ISERROR(SEARCH(".",J3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="12" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",J3)))</formula>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="containsText" dxfId="87" priority="12" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",K8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="11" operator="containsText" text=".">
+      <formula>NOT(ISERROR(SEARCH(".",K8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="10" operator="containsText" text="MI">
+      <formula>NOT(ISERROR(SEARCH("MI",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="containsText" dxfId="78" priority="7" operator="containsText" text="KI">
-      <formula>NOT(ISERROR(SEARCH("KI",K3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="8" operator="containsText" text=".">
-      <formula>NOT(ISERROR(SEARCH(".",K3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="9" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",K3)))</formula>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="containsText" dxfId="84" priority="9" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="8" operator="containsText" text=".">
+      <formula>NOT(ISERROR(SEARCH(".",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="7" operator="containsText" text="MI">
+      <formula>NOT(ISERROR(SEARCH("MI",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L20">
+    <cfRule type="containsText" dxfId="81" priority="18" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",L3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="16" operator="containsText" text="SA">
+      <formula>NOT(ISERROR(SEARCH("SA",L3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="17" operator="containsText" text=".">
+      <formula>NOT(ISERROR(SEARCH(".",L3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M20">
+    <cfRule type="containsText" dxfId="78" priority="13" operator="containsText" text="KI">
+      <formula>NOT(ISERROR(SEARCH("KI",M3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="15" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",M3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="14" operator="containsText" text=".">
+      <formula>NOT(ISERROR(SEARCH(".",M3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4158,30 +4318,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2492B5-5286-4C51-A0EE-617DAAF7402C}">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="11.375" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
-    <col min="4" max="4" width="7.25" customWidth="1"/>
-    <col min="5" max="5" width="16.75" customWidth="1"/>
-    <col min="6" max="6" width="47.75" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" customWidth="1"/>
+    <col min="3" max="3" width="9.8984375" customWidth="1"/>
+    <col min="4" max="4" width="7.19921875" customWidth="1"/>
+    <col min="5" max="5" width="16.69921875" customWidth="1"/>
+    <col min="6" max="6" width="47.69921875" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="11.625" customWidth="1"/>
-    <col min="9" max="9" width="8.125" customWidth="1"/>
-    <col min="10" max="10" width="13.75" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="12" width="14.25" customWidth="1"/>
-    <col min="13" max="13" width="16.375" customWidth="1"/>
-    <col min="14" max="14" width="15.75" customWidth="1"/>
+    <col min="8" max="8" width="11.59765625" customWidth="1"/>
+    <col min="9" max="9" width="8.09765625" customWidth="1"/>
+    <col min="10" max="10" width="11.59765625" customWidth="1"/>
+    <col min="11" max="11" width="8.09765625" customWidth="1"/>
+    <col min="12" max="12" width="13.69921875" customWidth="1"/>
+    <col min="13" max="13" width="12.69921875" customWidth="1"/>
+    <col min="14" max="14" width="14.19921875" customWidth="1"/>
+    <col min="15" max="15" width="16.3984375" customWidth="1"/>
+    <col min="16" max="16" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4207,31 +4369,37 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4239,7 +4407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="25.9" customHeight="1">
+    <row r="3" spans="1:18" ht="25.95" customHeight="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4259,7 +4427,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="31.15" customHeight="1">
+    <row r="4" spans="1:18" ht="31.2" customHeight="1">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4279,7 +4447,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="25.9" customHeight="1">
+    <row r="5" spans="1:18" ht="25.95" customHeight="1">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4298,11 +4466,11 @@
       <c r="H5" t="s">
         <v>267</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4322,7 +4490,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4341,8 +4509,11 @@
       <c r="H7" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="28.15" customHeight="1">
+      <c r="J7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="28.2" customHeight="1">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4362,7 +4533,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="30" customHeight="1">
+    <row r="9" spans="1:18" ht="30" customHeight="1">
       <c r="A9">
         <v>1</v>
       </c>
@@ -4382,7 +4553,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4402,7 +4573,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4422,7 +4593,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4442,7 +4613,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4462,7 +4633,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4475,11 +4646,11 @@
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:18">
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:18">
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>
     </row>
@@ -4731,22 +4902,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB6832A-6597-4EBE-A642-50EFC6AE260A}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="4" max="4" width="6.375" customWidth="1"/>
-    <col min="5" max="5" width="16.125" customWidth="1"/>
-    <col min="6" max="6" width="57.75" customWidth="1"/>
+    <col min="4" max="4" width="6.3984375" customWidth="1"/>
+    <col min="5" max="5" width="16.09765625" customWidth="1"/>
+    <col min="6" max="6" width="57.69921875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4772,31 +4944,37 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4804,7 +4982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4824,7 +5002,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4844,7 +5022,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4864,7 +5042,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4883,11 +5061,14 @@
       <c r="H6" t="s">
         <v>269</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="J6" t="s">
+        <v>274</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4907,7 +5088,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4927,7 +5108,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1</v>
       </c>
@@ -4947,7 +5128,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4967,7 +5148,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4987,7 +5168,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1</v>
       </c>
@@ -5006,8 +5187,11 @@
       <c r="H12" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="J12" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1</v>
       </c>
@@ -5027,7 +5211,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1</v>
       </c>
@@ -5047,7 +5231,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>0</v>
       </c>
@@ -5113,21 +5297,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4D3827-FA20-492E-9CAA-498828664590}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
-    <col min="6" max="6" width="52.75" customWidth="1"/>
-    <col min="7" max="7" width="19.625" customWidth="1"/>
-    <col min="8" max="8" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="15.3984375" customWidth="1"/>
+    <col min="6" max="6" width="52.69921875" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" customWidth="1"/>
+    <col min="8" max="8" width="11.59765625" customWidth="1"/>
+    <col min="10" max="10" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5153,31 +5338,37 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5185,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5205,7 +5396,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5225,7 +5416,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5245,7 +5436,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5265,7 +5456,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5284,11 +5475,11 @@
       <c r="H7" t="s">
         <v>220</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1</v>
       </c>
@@ -5308,7 +5499,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1</v>
       </c>
@@ -5328,7 +5519,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5348,7 +5539,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1</v>
       </c>
@@ -5368,7 +5559,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1</v>
       </c>
@@ -5388,7 +5579,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1</v>
       </c>
@@ -5408,7 +5599,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1</v>
       </c>
@@ -5428,7 +5619,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1</v>
       </c>
@@ -5447,8 +5638,11 @@
       <c r="H15" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="J15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1</v>
       </c>
@@ -5534,21 +5728,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E2E5F-C23B-4F25-A39B-FF9BDCB35635}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="F4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="14.09765625" customWidth="1"/>
     <col min="6" max="6" width="90" customWidth="1"/>
-    <col min="7" max="7" width="19.25" customWidth="1"/>
-    <col min="8" max="8" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="19.19921875" customWidth="1"/>
+    <col min="8" max="8" width="18.09765625" customWidth="1"/>
+    <col min="10" max="10" width="18.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5574,31 +5769,37 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5618,7 +5819,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5638,7 +5839,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5658,7 +5859,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5678,7 +5879,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5698,7 +5899,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5718,7 +5919,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1</v>
       </c>
@@ -5738,7 +5939,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1</v>
       </c>
@@ -5758,7 +5959,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5778,7 +5979,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1</v>
       </c>
@@ -5798,7 +5999,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1</v>
       </c>
@@ -5818,7 +6019,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1</v>
       </c>
@@ -5838,7 +6039,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1</v>
       </c>
@@ -5858,7 +6059,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1</v>
       </c>
@@ -5878,7 +6079,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1</v>
       </c>
@@ -5898,7 +6099,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>1</v>
       </c>
@@ -5918,7 +6119,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>1</v>
       </c>
@@ -5938,7 +6139,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>1</v>
       </c>
@@ -5958,7 +6159,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>1</v>
       </c>
@@ -5978,7 +6179,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5998,7 +6199,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>1</v>
       </c>
@@ -6018,7 +6219,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>1</v>
       </c>
@@ -6038,7 +6239,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>1</v>
       </c>
@@ -6058,7 +6259,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>1</v>
       </c>
@@ -6077,8 +6278,11 @@
       <c r="H25" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>0</v>
       </c>
@@ -6133,21 +6337,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57870A9-ECB4-4291-BFAF-986814B662D2}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="76.75" customWidth="1"/>
-    <col min="7" max="7" width="19.75" customWidth="1"/>
-    <col min="8" max="8" width="17.25" customWidth="1"/>
+    <col min="6" max="6" width="76.69921875" customWidth="1"/>
+    <col min="7" max="7" width="19.69921875" customWidth="1"/>
+    <col min="8" max="8" width="17.19921875" customWidth="1"/>
+    <col min="10" max="10" width="17.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6173,31 +6378,37 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6205,7 +6416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6221,8 +6432,11 @@
       <c r="G3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6239,7 +6453,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1</v>
       </c>
@@ -6256,7 +6470,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -6273,7 +6487,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1</v>
       </c>
@@ -6290,7 +6504,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1</v>
       </c>
@@ -6307,7 +6521,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1</v>
       </c>
@@ -6324,7 +6538,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1</v>
       </c>
@@ -6341,7 +6555,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1</v>
       </c>
@@ -6358,7 +6572,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1</v>
       </c>
@@ -6375,7 +6589,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1</v>
       </c>
@@ -6392,7 +6606,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1</v>
       </c>
@@ -6414,8 +6628,11 @@
       <c r="H14" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="J14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1</v>
       </c>
@@ -6435,7 +6652,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1</v>
       </c>
@@ -6454,8 +6671,11 @@
       <c r="H16" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="J16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>1</v>
       </c>
@@ -6475,7 +6695,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>1</v>
       </c>
@@ -6495,7 +6715,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>1</v>
       </c>
@@ -6515,7 +6735,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>1</v>
       </c>
@@ -6535,7 +6755,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="24">
+    <row r="21" spans="1:10" ht="26.4">
       <c r="A21">
         <v>1</v>
       </c>
@@ -6555,7 +6775,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>1</v>
       </c>
@@ -6575,7 +6795,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>1</v>
       </c>
@@ -6595,7 +6815,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>1</v>
       </c>
@@ -6615,7 +6835,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>1</v>
       </c>
@@ -6635,7 +6855,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>1</v>
       </c>
@@ -6655,7 +6875,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>1</v>
       </c>
@@ -6675,7 +6895,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>1</v>
       </c>
@@ -6695,7 +6915,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>1</v>
       </c>
@@ -6717,8 +6937,11 @@
       <c r="H29" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="J29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>1</v>
       </c>
@@ -6737,8 +6960,11 @@
       <c r="H30" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="J30" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>0</v>
       </c>
@@ -6793,21 +7019,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DD822B-AB3F-4083-911C-110C08E3FDA4}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView topLeftCell="B15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="55.5" customWidth="1"/>
-    <col min="7" max="7" width="22.375" customWidth="1"/>
-    <col min="8" max="8" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="22.3984375" customWidth="1"/>
+    <col min="8" max="8" width="11.59765625" customWidth="1"/>
+    <col min="10" max="10" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6833,31 +7060,37 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6865,7 +7098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6882,7 +7115,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6899,7 +7132,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1</v>
       </c>
@@ -6916,7 +7149,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -6936,7 +7169,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1</v>
       </c>
@@ -6956,7 +7189,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1</v>
       </c>
@@ -6973,7 +7206,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="24">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1</v>
       </c>
@@ -6990,7 +7223,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1</v>
       </c>
@@ -7007,7 +7240,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1</v>
       </c>
@@ -7024,7 +7257,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1</v>
       </c>
@@ -7041,7 +7274,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1</v>
       </c>
@@ -7058,7 +7291,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1</v>
       </c>
@@ -7078,7 +7311,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="24">
+    <row r="15" spans="1:18" ht="26.4">
       <c r="A15">
         <v>1</v>
       </c>
@@ -7098,7 +7331,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1</v>
       </c>
@@ -7115,7 +7348,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>1</v>
       </c>
@@ -7132,7 +7365,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>1</v>
       </c>
@@ -7149,7 +7382,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>1</v>
       </c>
@@ -7166,7 +7399,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>1</v>
       </c>
@@ -7183,7 +7416,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>1</v>
       </c>
@@ -7200,7 +7433,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>1</v>
       </c>
@@ -7217,7 +7450,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="24">
+    <row r="23" spans="1:10" ht="26.4">
       <c r="A23">
         <v>1</v>
       </c>
@@ -7234,7 +7467,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>1</v>
       </c>
@@ -7251,7 +7484,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>1</v>
       </c>
@@ -7268,7 +7501,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>1</v>
       </c>
@@ -7285,7 +7518,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>1</v>
       </c>
@@ -7302,7 +7535,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>1</v>
       </c>
@@ -7319,7 +7552,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>1</v>
       </c>
@@ -7338,8 +7571,11 @@
       <c r="H29" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="J29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>1</v>
       </c>
@@ -7359,7 +7595,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="24">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>1</v>
       </c>
@@ -7379,7 +7615,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>1</v>
       </c>
@@ -7399,7 +7635,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>1</v>
       </c>
@@ -7416,7 +7652,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>1</v>
       </c>
@@ -7433,7 +7669,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>1</v>
       </c>
@@ -7450,7 +7686,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>1</v>
       </c>
@@ -7467,7 +7703,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>1</v>
       </c>
@@ -7484,7 +7720,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>1</v>
       </c>
@@ -7501,7 +7737,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="24">
+    <row r="39" spans="1:9" ht="26.4">
       <c r="A39">
         <v>1</v>
       </c>
@@ -7517,8 +7753,11 @@
       <c r="G39" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>0</v>
       </c>
@@ -7573,24 +7812,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1151488-0F44-491C-8515-0B5CDD067839}">
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="10.8984375" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
     <col min="6" max="6" width="73.5" customWidth="1"/>
-    <col min="7" max="7" width="21.375" customWidth="1"/>
-    <col min="8" max="8" width="16.25" customWidth="1"/>
+    <col min="7" max="7" width="21.3984375" customWidth="1"/>
+    <col min="8" max="8" width="16.19921875" customWidth="1"/>
+    <col min="10" max="10" width="16.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7616,31 +7856,37 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7648,7 +7894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7665,7 +7911,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1</v>
       </c>
@@ -7682,7 +7928,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1</v>
       </c>
@@ -7699,7 +7945,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -7716,7 +7962,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1</v>
       </c>
@@ -7733,7 +7979,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1</v>
       </c>
@@ -7750,7 +7996,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1</v>
       </c>
@@ -7767,7 +8013,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1</v>
       </c>
@@ -7784,7 +8030,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1</v>
       </c>
@@ -7801,7 +8047,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1</v>
       </c>
@@ -7818,7 +8064,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1</v>
       </c>
@@ -7835,7 +8081,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1</v>
       </c>
@@ -7852,7 +8098,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1</v>
       </c>
@@ -7869,7 +8115,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1</v>
       </c>
@@ -7886,7 +8132,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>1</v>
       </c>
@@ -7903,7 +8149,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>1</v>
       </c>
@@ -7919,8 +8165,11 @@
       <c r="G18" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>1</v>
       </c>
@@ -7937,7 +8186,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>1</v>
       </c>
@@ -7954,7 +8203,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>1</v>
       </c>
@@ -7971,7 +8220,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>1</v>
       </c>
@@ -7988,7 +8237,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>1</v>
       </c>
@@ -8005,7 +8254,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>1</v>
       </c>
@@ -8022,7 +8271,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>1</v>
       </c>
@@ -8039,7 +8288,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>1</v>
       </c>
@@ -8056,7 +8305,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="24">
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>1</v>
       </c>
@@ -8073,7 +8322,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>1</v>
       </c>
@@ -8090,7 +8339,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>1</v>
       </c>
@@ -8107,7 +8356,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>1</v>
       </c>
@@ -8124,7 +8373,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>1</v>
       </c>
@@ -8141,7 +8390,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>1</v>
       </c>
@@ -8161,7 +8410,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>1</v>
       </c>
@@ -8181,7 +8430,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>1</v>
       </c>
@@ -8201,7 +8450,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>1</v>
       </c>
@@ -8220,8 +8469,11 @@
       <c r="H35" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="J35" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>1</v>
       </c>
@@ -8244,7 +8496,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>1</v>
       </c>
@@ -8267,7 +8519,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>1</v>
       </c>
@@ -8290,7 +8542,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>1</v>
       </c>
@@ -8313,7 +8565,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>1</v>
       </c>
@@ -8336,7 +8588,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>1</v>
       </c>
@@ -8359,7 +8611,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>1</v>
       </c>
@@ -8381,8 +8633,11 @@
       <c r="H42" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="J42" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>1</v>
       </c>
@@ -8405,7 +8660,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>1</v>
       </c>
@@ -8428,7 +8683,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>1</v>
       </c>
@@ -8451,7 +8706,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>1</v>
       </c>
@@ -8474,7 +8729,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>1</v>
       </c>
@@ -8497,7 +8752,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>1</v>
       </c>
@@ -8520,7 +8775,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>1</v>
       </c>
@@ -8543,7 +8798,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>1</v>
       </c>
@@ -8566,7 +8821,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>1</v>
       </c>
@@ -8586,7 +8841,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>1</v>
       </c>
@@ -8605,8 +8860,11 @@
       <c r="H52" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="J52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>1</v>
       </c>
@@ -8626,7 +8884,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>1</v>
       </c>
@@ -8646,7 +8904,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>1</v>
       </c>
@@ -8666,7 +8924,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="96">
+    <row r="56" spans="1:10" ht="92.4">
       <c r="A56">
         <v>1</v>
       </c>
@@ -8686,7 +8944,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>1</v>
       </c>
@@ -8706,7 +8964,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>1</v>
       </c>
@@ -8725,8 +8983,11 @@
       <c r="H58" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="J58" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>1</v>
       </c>
@@ -8745,8 +9006,11 @@
       <c r="H59" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="J59" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>1</v>
       </c>
@@ -8766,7 +9030,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>1</v>
       </c>
@@ -8786,7 +9050,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>1</v>
       </c>
@@ -8806,7 +9070,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>1</v>
       </c>
@@ -8826,7 +9090,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>1</v>
       </c>
@@ -8846,7 +9110,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>1</v>
       </c>
@@ -8865,8 +9129,11 @@
       <c r="H65" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="J65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>1</v>
       </c>
@@ -8886,7 +9153,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>1</v>
       </c>
@@ -8906,7 +9173,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>1</v>
       </c>
@@ -8926,7 +9193,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>1</v>
       </c>
@@ -8946,7 +9213,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>1</v>
       </c>
@@ -8966,7 +9233,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>1</v>
       </c>
@@ -8986,7 +9253,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>1</v>
       </c>
@@ -9006,7 +9273,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>1</v>
       </c>
@@ -9026,7 +9293,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>1</v>
       </c>
@@ -9045,8 +9312,11 @@
       <c r="H74" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="J74">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>1</v>
       </c>
@@ -9065,8 +9335,11 @@
       <c r="H75" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="J75" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>1</v>
       </c>
@@ -9086,7 +9359,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>1</v>
       </c>
@@ -9106,7 +9379,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>1</v>
       </c>
@@ -9126,7 +9399,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="48">
+    <row r="79" spans="1:10" ht="39.6">
       <c r="A79">
         <v>1</v>
       </c>
@@ -9146,7 +9419,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>1</v>
       </c>
@@ -9165,8 +9438,11 @@
       <c r="H80" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="81" spans="1:16">
+      <c r="J80">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
       <c r="A81">
         <v>1</v>
       </c>
@@ -9185,8 +9461,11 @@
       <c r="H81" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" ht="96">
+      <c r="J81">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="105.6">
       <c r="A82">
         <v>1</v>
       </c>
@@ -9206,7 +9485,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:18">
       <c r="A83">
         <v>1</v>
       </c>
@@ -9226,7 +9505,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:18">
       <c r="A84">
         <v>1</v>
       </c>
@@ -9246,7 +9525,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:18">
       <c r="A85">
         <v>1</v>
       </c>
@@ -9266,7 +9545,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:18">
       <c r="A86">
         <v>1</v>
       </c>
@@ -9282,12 +9561,15 @@
       <c r="G86" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="87" spans="1:16">
+      <c r="I86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
       <c r="A87">
         <v>2</v>
       </c>
-      <c r="P87">
+      <c r="R87">
         <v>4</v>
       </c>
     </row>

</xml_diff>